<commit_message>
add some new data sets, collected more data points for P-V relationships
</commit_message>
<xml_diff>
--- a/PVdata.xlsx
+++ b/PVdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -57,7 +57,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -89,11 +89,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -221,14 +216,14 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <c:chart>
     <c:plotArea>
       <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
+        <c:scatterStyle val="line"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -256,16 +251,9 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="square"/>
-            <c:size val="8"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="004586"/>
-              </a:solidFill>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
-            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -286,10 +274,10 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$G$2:$G$19</c:f>
+              <c:f>Sheet1!$G$2:$G$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>0.000351864883884588</c:v>
                 </c:pt>
@@ -342,17 +330,38 @@
                   <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>0.212765957446808</c:v>
+                </c:pt>
+                <c:pt idx="18">
                   <c:v>0.227272727272727</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.238095238095238</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.266666666666667</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.285714285714286</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.307692307692308</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.333333333333333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$19</c:f>
+              <c:f>Sheet1!$B$2:$B$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>2.77</c:v>
                 </c:pt>
@@ -360,52 +369,73 @@
                   <c:v>10.26</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>67.5</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>103</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>185</c:v>
+                  <c:v>197</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>414</c:v>
+                  <c:v>452</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>633</c:v>
+                  <c:v>730</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1030</c:v>
+                  <c:v>1255</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1180</c:v>
+                  <c:v>1450</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1600</c:v>
+                  <c:v>2050</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2400</c:v>
+                  <c:v>3280</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2930</c:v>
+                  <c:v>4170</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3940</c:v>
+                  <c:v>5925</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4285</c:v>
+                  <c:v>6520</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4990</c:v>
+                  <c:v>7835</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5360</c:v>
+                  <c:v>8550</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6380</c:v>
+                  <c:v>10590</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8645</c:v>
+                  <c:v>12430</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>14860</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>16900</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>19130</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>23000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>27550</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>33000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>40000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -438,16 +468,9 @@
             </a:ln>
           </c:spPr>
           <c:marker>
-            <c:symbol val="diamond"/>
-            <c:size val="8"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
-            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -468,73 +491,94 @@
           </c:dLbls>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$H$2:$H$19</c:f>
+              <c:f>Sheet1!$H$2:$H$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>0.000352219762372657</c:v>
+                  <c:v>0.000352148962352698</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.00130439907104098</c:v>
+                  <c:v>0.00130342858125705</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.00853704521656788</c:v>
+                  <c:v>0.00849564551485895</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0129640233616497</c:v>
+                  <c:v>0.0128687939938936</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0221549954953953</c:v>
+                  <c:v>0.0218783148491767</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0451741633755441</c:v>
+                  <c:v>0.0440385859992941</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0660652648500316</c:v>
+                  <c:v>0.0636644246928005</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0986529219265749</c:v>
+                  <c:v>0.0933937082076311</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.10945053723083</c:v>
+                  <c:v>0.103014626142723</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.140123784135787</c:v>
+                  <c:v>0.129746122812774</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.194683307702471</c:v>
+                  <c:v>0.175212375625125</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.230598204694633</c:v>
+                  <c:v>0.203775578136928</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.295286006521082</c:v>
+                  <c:v>0.252693752957386</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.318821919360952</c:v>
+                  <c:v>0.269733762119723</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.365423990584417</c:v>
+                  <c:v>0.302356011962149</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.393398364700391</c:v>
+                  <c:v>0.321257807999922</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.468044889321525</c:v>
+                  <c:v>0.369363593889636</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.650809813637529</c:v>
+                  <c:v>0.415392897993352</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.474527504585557</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.524285038817918</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.585699763462427</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.686172536550428</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.828253787040738</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.04453979786481</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.41370849400737</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$19</c:f>
+              <c:f>Sheet1!$B$2:$B$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="18"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>2.77</c:v>
                 </c:pt>
@@ -542,63 +586,84 @@
                   <c:v>10.26</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>67.5</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>103</c:v>
+                  <c:v>110</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>185</c:v>
+                  <c:v>197</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>414</c:v>
+                  <c:v>452</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>633</c:v>
+                  <c:v>730</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1030</c:v>
+                  <c:v>1255</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1180</c:v>
+                  <c:v>1450</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1600</c:v>
+                  <c:v>2050</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2400</c:v>
+                  <c:v>3280</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2930</c:v>
+                  <c:v>4170</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3940</c:v>
+                  <c:v>5925</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4285</c:v>
+                  <c:v>6520</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4990</c:v>
+                  <c:v>7835</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5360</c:v>
+                  <c:v>8550</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>6380</c:v>
+                  <c:v>10590</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8645</c:v>
+                  <c:v>12430</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>14860</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>16900</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>19130</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>23000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>27550</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>33000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>40000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="31018388"/>
-        <c:axId val="60528618"/>
+        <c:axId val="49855205"/>
+        <c:axId val="51720315"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="31018388"/>
+        <c:axId val="49855205"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -613,34 +678,6 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>1/V</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -663,12 +700,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60528618"/>
+        <c:crossAx val="51720315"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="60528618"/>
+        <c:axId val="51720315"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -683,34 +720,6 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>P</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
@@ -733,7 +742,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="31018388"/>
+        <c:crossAx val="49855205"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -785,16 +794,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>30240</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>36360</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>65880</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>65880</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>67320</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>48240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -802,8 +811,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3281400" y="0"/>
-        <a:ext cx="7350840" cy="6405480"/>
+        <a:off x="6350760" y="0"/>
+        <a:ext cx="7619040" cy="6458400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -837,10 +846,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G27" activeCellId="0" sqref="G27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F32" activeCellId="0" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -891,7 +900,7 @@
       </c>
       <c r="D2" s="0" t="n">
         <f aca="false">C2-$I$2</f>
-        <v>2839.1365472048</v>
+        <v>2839.70735940559</v>
       </c>
       <c r="E2" s="0" t="n">
         <f aca="false">B2*C2</f>
@@ -907,11 +916,11 @@
       </c>
       <c r="H2" s="0" t="n">
         <f aca="false">1/(C2-$I$2)</f>
-        <v>0.000352219762372657</v>
+        <v>0.000352148962352698</v>
       </c>
       <c r="I2" s="0" t="n">
-        <f aca="false">4/3*0.07^3*1993*PI()</f>
-        <v>2.86345279520177</v>
+        <f aca="false">4/3*0.065^3*1993*PI()</f>
+        <v>2.292640594409</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -926,7 +935,7 @@
       </c>
       <c r="D3" s="0" t="n">
         <f aca="false">C3-$I$2</f>
-        <v>766.636547204798</v>
+        <v>767.207359405591</v>
       </c>
       <c r="E3" s="0" t="n">
         <f aca="false">B3*C3</f>
@@ -942,7 +951,7 @@
       </c>
       <c r="H3" s="0" t="n">
         <f aca="false">1/(C3-$I$2)</f>
-        <v>0.00130439907104098</v>
+        <v>0.00130342858125705</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -950,22 +959,22 @@
         <v>7700</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>67.5</v>
+        <v>70</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>120</v>
       </c>
       <c r="D4" s="0" t="n">
         <f aca="false">C4-$I$2</f>
-        <v>117.136547204798</v>
+        <v>117.707359405591</v>
       </c>
       <c r="E4" s="0" t="n">
         <f aca="false">B4*C4</f>
-        <v>8100</v>
+        <v>8400</v>
       </c>
       <c r="F4" s="0" t="n">
         <f aca="false">E4/A4</f>
-        <v>1.05194805194805</v>
+        <v>1.09090909090909</v>
       </c>
       <c r="G4" s="0" t="n">
         <f aca="false">1/C4</f>
@@ -973,7 +982,7 @@
       </c>
       <c r="H4" s="0" t="n">
         <f aca="false">1/(C4-$I$2)</f>
-        <v>0.00853704521656788</v>
+        <v>0.00849564551485895</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -981,22 +990,22 @@
         <v>7700</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>80</v>
       </c>
       <c r="D5" s="0" t="n">
         <f aca="false">C5-$I$2</f>
-        <v>77.1365472047982</v>
+        <v>77.707359405591</v>
       </c>
       <c r="E5" s="0" t="n">
         <f aca="false">B5*C5</f>
-        <v>8240</v>
+        <v>8800</v>
       </c>
       <c r="F5" s="0" t="n">
         <f aca="false">E5/A5</f>
-        <v>1.07012987012987</v>
+        <v>1.14285714285714</v>
       </c>
       <c r="G5" s="0" t="n">
         <f aca="false">1/C5</f>
@@ -1004,7 +1013,7 @@
       </c>
       <c r="H5" s="0" t="n">
         <f aca="false">1/(C5-$I$2)</f>
-        <v>0.0129640233616497</v>
+        <v>0.0128687939938936</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1012,22 +1021,22 @@
         <v>7700</v>
       </c>
       <c r="B6" s="0" t="n">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>48</v>
       </c>
       <c r="D6" s="0" t="n">
         <f aca="false">C6-$I$2</f>
-        <v>45.1365472047982</v>
+        <v>45.707359405591</v>
       </c>
       <c r="E6" s="0" t="n">
         <f aca="false">B6*C6</f>
-        <v>8880</v>
+        <v>9456</v>
       </c>
       <c r="F6" s="0" t="n">
         <f aca="false">E6/A6</f>
-        <v>1.15324675324675</v>
+        <v>1.22805194805195</v>
       </c>
       <c r="G6" s="0" t="n">
         <f aca="false">1/C6</f>
@@ -1035,7 +1044,7 @@
       </c>
       <c r="H6" s="0" t="n">
         <f aca="false">1/(C6-$I$2)</f>
-        <v>0.0221549954953953</v>
+        <v>0.0218783148491767</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1043,22 +1052,22 @@
         <v>7800</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>414</v>
+        <v>452</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>25</v>
       </c>
       <c r="D7" s="0" t="n">
         <f aca="false">C7-$I$2</f>
-        <v>22.1365472047982</v>
+        <v>22.707359405591</v>
       </c>
       <c r="E7" s="0" t="n">
         <f aca="false">B7*C7</f>
-        <v>10350</v>
+        <v>11300</v>
       </c>
       <c r="F7" s="0" t="n">
         <f aca="false">E7/A7</f>
-        <v>1.32692307692308</v>
+        <v>1.44871794871795</v>
       </c>
       <c r="G7" s="0" t="n">
         <f aca="false">1/C7</f>
@@ -1066,7 +1075,7 @@
       </c>
       <c r="H7" s="0" t="n">
         <f aca="false">1/(C7-$I$2)</f>
-        <v>0.0451741633755441</v>
+        <v>0.0440385859992941</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1074,22 +1083,22 @@
         <v>7700</v>
       </c>
       <c r="B8" s="0" t="n">
-        <v>633</v>
+        <v>730</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>18</v>
       </c>
       <c r="D8" s="0" t="n">
         <f aca="false">C8-$I$2</f>
-        <v>15.1365472047982</v>
+        <v>15.707359405591</v>
       </c>
       <c r="E8" s="0" t="n">
         <f aca="false">B8*C8</f>
-        <v>11394</v>
+        <v>13140</v>
       </c>
       <c r="F8" s="0" t="n">
         <f aca="false">E8/A8</f>
-        <v>1.47974025974026</v>
+        <v>1.70649350649351</v>
       </c>
       <c r="G8" s="0" t="n">
         <f aca="false">1/C8</f>
@@ -1097,7 +1106,7 @@
       </c>
       <c r="H8" s="0" t="n">
         <f aca="false">1/(C8-$I$2)</f>
-        <v>0.0660652648500316</v>
+        <v>0.0636644246928005</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1105,22 +1114,22 @@
         <v>7700</v>
       </c>
       <c r="B9" s="0" t="n">
-        <v>1030</v>
+        <v>1255</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>13</v>
       </c>
       <c r="D9" s="0" t="n">
         <f aca="false">C9-$I$2</f>
-        <v>10.1365472047982</v>
+        <v>10.707359405591</v>
       </c>
       <c r="E9" s="0" t="n">
         <f aca="false">B9*C9</f>
-        <v>13390</v>
+        <v>16315</v>
       </c>
       <c r="F9" s="0" t="n">
         <f aca="false">E9/A9</f>
-        <v>1.73896103896104</v>
+        <v>2.11883116883117</v>
       </c>
       <c r="G9" s="0" t="n">
         <f aca="false">1/C9</f>
@@ -1128,7 +1137,7 @@
       </c>
       <c r="H9" s="0" t="n">
         <f aca="false">1/(C9-$I$2)</f>
-        <v>0.0986529219265749</v>
+        <v>0.0933937082076311</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1136,22 +1145,22 @@
         <v>7700</v>
       </c>
       <c r="B10" s="0" t="n">
-        <v>1180</v>
+        <v>1450</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>12</v>
       </c>
       <c r="D10" s="0" t="n">
         <f aca="false">C10-$I$2</f>
-        <v>9.13654720479823</v>
+        <v>9.707359405591</v>
       </c>
       <c r="E10" s="0" t="n">
         <f aca="false">B10*C10</f>
-        <v>14160</v>
+        <v>17400</v>
       </c>
       <c r="F10" s="0" t="n">
         <f aca="false">E10/A10</f>
-        <v>1.83896103896104</v>
+        <v>2.25974025974026</v>
       </c>
       <c r="G10" s="0" t="n">
         <f aca="false">1/C10</f>
@@ -1159,7 +1168,7 @@
       </c>
       <c r="H10" s="0" t="n">
         <f aca="false">1/(C10-$I$2)</f>
-        <v>0.10945053723083</v>
+        <v>0.103014626142723</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1167,22 +1176,22 @@
         <v>7700</v>
       </c>
       <c r="B11" s="0" t="n">
-        <v>1600</v>
+        <v>2050</v>
       </c>
       <c r="C11" s="0" t="n">
         <v>10</v>
       </c>
       <c r="D11" s="0" t="n">
         <f aca="false">C11-$I$2</f>
-        <v>7.13654720479823</v>
+        <v>7.707359405591</v>
       </c>
       <c r="E11" s="0" t="n">
         <f aca="false">B11*C11</f>
-        <v>16000</v>
+        <v>20500</v>
       </c>
       <c r="F11" s="0" t="n">
         <f aca="false">E11/A11</f>
-        <v>2.07792207792208</v>
+        <v>2.66233766233766</v>
       </c>
       <c r="G11" s="0" t="n">
         <f aca="false">1/C11</f>
@@ -1190,7 +1199,7 @@
       </c>
       <c r="H11" s="0" t="n">
         <f aca="false">1/(C11-$I$2)</f>
-        <v>0.140123784135787</v>
+        <v>0.129746122812774</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1198,22 +1207,22 @@
         <v>7700</v>
       </c>
       <c r="B12" s="0" t="n">
-        <v>2400</v>
+        <v>3280</v>
       </c>
       <c r="C12" s="0" t="n">
         <v>8</v>
       </c>
       <c r="D12" s="0" t="n">
         <f aca="false">C12-$I$2</f>
-        <v>5.13654720479823</v>
+        <v>5.707359405591</v>
       </c>
       <c r="E12" s="0" t="n">
         <f aca="false">B12*C12</f>
-        <v>19200</v>
+        <v>26240</v>
       </c>
       <c r="F12" s="0" t="n">
         <f aca="false">E12/A12</f>
-        <v>2.49350649350649</v>
+        <v>3.40779220779221</v>
       </c>
       <c r="G12" s="0" t="n">
         <f aca="false">1/C12</f>
@@ -1221,7 +1230,7 @@
       </c>
       <c r="H12" s="0" t="n">
         <f aca="false">1/(C12-$I$2)</f>
-        <v>0.194683307702471</v>
+        <v>0.175212375625125</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1229,22 +1238,22 @@
         <v>7700</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>2930</v>
+        <v>4170</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>7.2</v>
       </c>
       <c r="D13" s="0" t="n">
         <f aca="false">C13-$I$2</f>
-        <v>4.33654720479823</v>
+        <v>4.907359405591</v>
       </c>
       <c r="E13" s="0" t="n">
         <f aca="false">B13*C13</f>
-        <v>21096</v>
+        <v>30024</v>
       </c>
       <c r="F13" s="0" t="n">
         <f aca="false">E13/A13</f>
-        <v>2.73974025974026</v>
+        <v>3.89922077922078</v>
       </c>
       <c r="G13" s="0" t="n">
         <f aca="false">1/C13</f>
@@ -1252,7 +1261,7 @@
       </c>
       <c r="H13" s="0" t="n">
         <f aca="false">1/(C13-$I$2)</f>
-        <v>0.230598204694633</v>
+        <v>0.203775578136928</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1260,22 +1269,22 @@
         <v>7700</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>3940</v>
+        <v>5925</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>6.25</v>
       </c>
       <c r="D14" s="0" t="n">
         <f aca="false">C14-$I$2</f>
-        <v>3.38654720479823</v>
+        <v>3.957359405591</v>
       </c>
       <c r="E14" s="0" t="n">
         <f aca="false">B14*C14</f>
-        <v>24625</v>
+        <v>37031.25</v>
       </c>
       <c r="F14" s="0" t="n">
         <f aca="false">E14/A14</f>
-        <v>3.19805194805195</v>
+        <v>4.80925324675325</v>
       </c>
       <c r="G14" s="0" t="n">
         <f aca="false">1/C14</f>
@@ -1283,7 +1292,7 @@
       </c>
       <c r="H14" s="0" t="n">
         <f aca="false">1/(C14-$I$2)</f>
-        <v>0.295286006521082</v>
+        <v>0.252693752957386</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1291,22 +1300,22 @@
         <v>7700</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>4285</v>
+        <v>6520</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>6</v>
       </c>
       <c r="D15" s="0" t="n">
         <f aca="false">C15-$I$2</f>
-        <v>3.13654720479823</v>
+        <v>3.707359405591</v>
       </c>
       <c r="E15" s="0" t="n">
         <f aca="false">B15*C15</f>
-        <v>25710</v>
+        <v>39120</v>
       </c>
       <c r="F15" s="0" t="n">
         <f aca="false">E15/A15</f>
-        <v>3.33896103896104</v>
+        <v>5.08051948051948</v>
       </c>
       <c r="G15" s="0" t="n">
         <f aca="false">1/C15</f>
@@ -1314,7 +1323,7 @@
       </c>
       <c r="H15" s="0" t="n">
         <f aca="false">1/(C15-$I$2)</f>
-        <v>0.318821919360952</v>
+        <v>0.269733762119723</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1322,22 +1331,22 @@
         <v>7700</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>4990</v>
+        <v>7835</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>5.6</v>
       </c>
       <c r="D16" s="0" t="n">
         <f aca="false">C16-$I$2</f>
-        <v>2.73654720479823</v>
+        <v>3.307359405591</v>
       </c>
       <c r="E16" s="0" t="n">
         <f aca="false">B16*C16</f>
-        <v>27944</v>
+        <v>43876</v>
       </c>
       <c r="F16" s="0" t="n">
         <f aca="false">E16/A16</f>
-        <v>3.62909090909091</v>
+        <v>5.69818181818182</v>
       </c>
       <c r="G16" s="0" t="n">
         <f aca="false">1/C16</f>
@@ -1345,7 +1354,7 @@
       </c>
       <c r="H16" s="0" t="n">
         <f aca="false">1/(C16-$I$2)</f>
-        <v>0.365423990584417</v>
+        <v>0.302356011962149</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1353,7 +1362,7 @@
         <v>7700</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>5360</v>
+        <v>8550</v>
       </c>
       <c r="C17" s="0" t="n">
         <f aca="false">200/37</f>
@@ -1361,15 +1370,15 @@
       </c>
       <c r="D17" s="0" t="n">
         <f aca="false">C17-$I$2</f>
-        <v>2.54195261020363</v>
+        <v>3.11276481099641</v>
       </c>
       <c r="E17" s="0" t="n">
         <f aca="false">B17*C17</f>
-        <v>28972.972972973</v>
+        <v>46216.2162162162</v>
       </c>
       <c r="F17" s="0" t="n">
         <f aca="false">E17/A17</f>
-        <v>3.76272376272376</v>
+        <v>6.00210600210601</v>
       </c>
       <c r="G17" s="0" t="n">
         <f aca="false">1/C17</f>
@@ -1377,7 +1386,7 @@
       </c>
       <c r="H17" s="0" t="n">
         <f aca="false">1/(C17-$I$2)</f>
-        <v>0.393398364700391</v>
+        <v>0.321257807999922</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1385,22 +1394,22 @@
         <v>7700</v>
       </c>
       <c r="B18" s="0" t="n">
-        <v>6380</v>
+        <v>10590</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>5</v>
       </c>
       <c r="D18" s="0" t="n">
         <f aca="false">C18-$I$2</f>
-        <v>2.13654720479823</v>
+        <v>2.707359405591</v>
       </c>
       <c r="E18" s="0" t="n">
         <f aca="false">B18*C18</f>
-        <v>31900</v>
+        <v>52950</v>
       </c>
       <c r="F18" s="0" t="n">
         <f aca="false">E18/A18</f>
-        <v>4.14285714285714</v>
+        <v>6.87662337662338</v>
       </c>
       <c r="G18" s="0" t="n">
         <f aca="false">1/C18</f>
@@ -1408,7 +1417,7 @@
       </c>
       <c r="H18" s="0" t="n">
         <f aca="false">1/(C18-$I$2)</f>
-        <v>0.468044889321525</v>
+        <v>0.369363593889636</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1416,30 +1425,247 @@
         <v>7700</v>
       </c>
       <c r="B19" s="0" t="n">
-        <v>8645</v>
+        <v>12430</v>
       </c>
       <c r="C19" s="0" t="n">
-        <v>4.4</v>
+        <v>4.7</v>
       </c>
       <c r="D19" s="0" t="n">
         <f aca="false">C19-$I$2</f>
-        <v>1.53654720479823</v>
+        <v>2.407359405591</v>
       </c>
       <c r="E19" s="0" t="n">
         <f aca="false">B19*C19</f>
-        <v>38038</v>
+        <v>58421</v>
       </c>
       <c r="F19" s="0" t="n">
         <f aca="false">E19/A19</f>
-        <v>4.94</v>
+        <v>7.58714285714286</v>
       </c>
       <c r="G19" s="0" t="n">
         <f aca="false">1/C19</f>
-        <v>0.227272727272727</v>
+        <v>0.212765957446808</v>
       </c>
       <c r="H19" s="0" t="n">
         <f aca="false">1/(C19-$I$2)</f>
-        <v>0.650809813637529</v>
+        <v>0.415392897993352</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>7700</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>14860</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <f aca="false">C20-$I$2</f>
+        <v>2.107359405591</v>
+      </c>
+      <c r="E20" s="0" t="n">
+        <f aca="false">B20*C20</f>
+        <v>65384</v>
+      </c>
+      <c r="F20" s="0" t="n">
+        <f aca="false">E20/A20</f>
+        <v>8.49142857142857</v>
+      </c>
+      <c r="G20" s="0" t="n">
+        <f aca="false">1/C20</f>
+        <v>0.227272727272727</v>
+      </c>
+      <c r="H20" s="0" t="n">
+        <f aca="false">1/(C20-$I$2)</f>
+        <v>0.474527504585557</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>7700</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>16900</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <f aca="false">C21-$I$2</f>
+        <v>1.907359405591</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <f aca="false">B21*C21</f>
+        <v>70980</v>
+      </c>
+      <c r="F21" s="0" t="n">
+        <f aca="false">E21/A21</f>
+        <v>9.21818181818182</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <f aca="false">1/C21</f>
+        <v>0.238095238095238</v>
+      </c>
+      <c r="H21" s="0" t="n">
+        <f aca="false">1/(C21-$I$2)</f>
+        <v>0.524285038817918</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>7700</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>19130</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <f aca="false">C22-$I$2</f>
+        <v>1.707359405591</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <f aca="false">B22*C22</f>
+        <v>76520</v>
+      </c>
+      <c r="F22" s="0" t="n">
+        <f aca="false">E22/A22</f>
+        <v>9.93766233766234</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <f aca="false">1/C22</f>
+        <v>0.25</v>
+      </c>
+      <c r="H22" s="0" t="n">
+        <f aca="false">1/(C22-$I$2)</f>
+        <v>0.585699763462427</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>7700</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>23000</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>3.75</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <f aca="false">C23-$I$2</f>
+        <v>1.457359405591</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <f aca="false">B23*C23</f>
+        <v>86250</v>
+      </c>
+      <c r="F23" s="0" t="n">
+        <f aca="false">E23/A23</f>
+        <v>11.2012987012987</v>
+      </c>
+      <c r="G23" s="0" t="n">
+        <f aca="false">1/C23</f>
+        <v>0.266666666666667</v>
+      </c>
+      <c r="H23" s="0" t="n">
+        <f aca="false">1/(C23-$I$2)</f>
+        <v>0.686172536550428</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>7700</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>27550</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <f aca="false">C24-$I$2</f>
+        <v>1.207359405591</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <f aca="false">B24*C24</f>
+        <v>96425</v>
+      </c>
+      <c r="F24" s="0" t="n">
+        <f aca="false">E24/A24</f>
+        <v>12.5227272727273</v>
+      </c>
+      <c r="G24" s="0" t="n">
+        <f aca="false">1/C24</f>
+        <v>0.285714285714286</v>
+      </c>
+      <c r="H24" s="0" t="n">
+        <f aca="false">1/(C24-$I$2)</f>
+        <v>0.828253787040738</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>7700</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>33000</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>3.25</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <f aca="false">C25-$I$2</f>
+        <v>0.957359405591</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <f aca="false">B25*C25</f>
+        <v>107250</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <f aca="false">E25/A25</f>
+        <v>13.9285714285714</v>
+      </c>
+      <c r="G25" s="0" t="n">
+        <f aca="false">1/C25</f>
+        <v>0.307692307692308</v>
+      </c>
+      <c r="H25" s="0" t="n">
+        <f aca="false">1/(C25-$I$2)</f>
+        <v>1.04453979786481</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>7700</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>40000</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <f aca="false">C26-$I$2</f>
+        <v>0.707359405591001</v>
+      </c>
+      <c r="E26" s="0" t="n">
+        <f aca="false">B26*C26</f>
+        <v>120000</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <f aca="false">E26/A26</f>
+        <v>15.5844155844156</v>
+      </c>
+      <c r="G26" s="0" t="n">
+        <f aca="false">1/C26</f>
+        <v>0.333333333333333</v>
+      </c>
+      <c r="H26" s="0" t="n">
+        <f aca="false">1/(C26-$I$2)</f>
+        <v>1.41370849400737</v>
       </c>
     </row>
   </sheetData>
@@ -1450,8 +1676,9 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
+  <drawing r:id="rId1"/>
   <tableParts>
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1463,8 +1690,8 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J15" activeCellId="0" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1479,6 +1706,5 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added random initial velocity, make average tools print more info
</commit_message>
<xml_diff>
--- a/PVdata.xlsx
+++ b/PVdata.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">NkT</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t xml:space="preserve">PV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P(V-A)</t>
   </si>
   <si>
     <t xml:space="preserve">ratio</t>
@@ -57,13 +60,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -81,11 +83,87 @@
       <family val="0"/>
     </font>
     <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i val="true"/>
+      <sz val="10"/>
+      <color rgb="FF808080"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color rgb="FF0000EE"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF996600"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCC0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -93,15 +171,57 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FF800000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF000000"/>
+        <bgColor rgb="FF003300"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF808080"/>
+        <bgColor rgb="FF969696"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -109,8 +229,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin">
+        <color rgb="FF808080"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF808080"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF808080"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF808080"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -134,39 +269,107 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="23">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Heading" xfId="20"/>
+    <cellStyle name="Heading 1" xfId="21"/>
+    <cellStyle name="Heading 2" xfId="22"/>
+    <cellStyle name="Text" xfId="23"/>
+    <cellStyle name="Note" xfId="24"/>
+    <cellStyle name="Footnote" xfId="25"/>
+    <cellStyle name="Hyperlink" xfId="26"/>
+    <cellStyle name="Status" xfId="27"/>
+    <cellStyle name="Good" xfId="28"/>
+    <cellStyle name="Neutral" xfId="29"/>
+    <cellStyle name="Bad" xfId="30"/>
+    <cellStyle name="Warning" xfId="31"/>
+    <cellStyle name="Error" xfId="32"/>
+    <cellStyle name="Accent" xfId="33"/>
+    <cellStyle name="Accent 1" xfId="34"/>
+    <cellStyle name="Accent 2" xfId="35"/>
+    <cellStyle name="Accent 3" xfId="36"/>
   </cellStyles>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFCC0000"/>
       <rgbColor rgb="FF00FF00"/>
-      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF0000EE"/>
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
-      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF006600"/>
       <rgbColor rgb="FF000080"/>
-      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF996600"/>
       <rgbColor rgb="FF800080"/>
       <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFB3B3B3"/>
@@ -178,7 +381,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -194,7 +397,7 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFFCCCC"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -216,7 +419,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -230,7 +433,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$G$1</c:f>
+              <c:f>Sheet1!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -254,223 +457,7 @@
             <c:symbol val="none"/>
           </c:marker>
           <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
-          <c:xVal>
-            <c:numRef>
-              <c:f>Sheet1!$G$2:$G$26</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
-                <c:pt idx="0">
-                  <c:v>0.000351864883884588</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.00129954515919428</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.00833333333333333</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.0125</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.0208333333333333</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.04</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.0555555555555556</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.0769230769230769</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.0833333333333333</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.1</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.125</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.138888888888889</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.16</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.166666666666667</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.178571428571429</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.185</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>0.2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>0.212765957446808</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>0.227272727272727</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>0.238095238095238</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.25</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>0.266666666666667</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>0.285714285714286</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>0.307692307692308</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>0.333333333333333</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$B$2:$B$26</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="25"/>
-                <c:pt idx="0">
-                  <c:v>2.77</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>10.26</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>70</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>110</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>197</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>452</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>730</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1255</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1450</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2050</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3280</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>4170</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>5925</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>6520</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>7835</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>8550</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>10590</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>12430</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>14860</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>16900</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>19130</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>23000</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>27550</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>33000</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>40000</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$H$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>1/(V-A)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="ff420e"/>
-            </a:solidFill>
-            <a:ln w="28800">
-              <a:solidFill>
-                <a:srgbClr val="ff420e"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:txPr>
               <a:bodyPr/>
               <a:lstStyle/>
@@ -496,79 +483,79 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>0.000352148962352698</c:v>
+                  <c:v>0.000351864883884588</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.00130342858125705</c:v>
+                  <c:v>0.00129954515919428</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.00849564551485895</c:v>
+                  <c:v>0.00833333333333333</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0128687939938936</c:v>
+                  <c:v>0.0125</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0218783148491767</c:v>
+                  <c:v>0.0208333333333333</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0440385859992941</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0636644246928005</c:v>
+                  <c:v>0.0555555555555556</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0933937082076311</c:v>
+                  <c:v>0.0769230769230769</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.103014626142723</c:v>
+                  <c:v>0.0833333333333333</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.129746122812774</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.175212375625125</c:v>
+                  <c:v>0.125</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.203775578136928</c:v>
+                  <c:v>0.138888888888889</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.252693752957386</c:v>
+                  <c:v>0.16</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.269733762119723</c:v>
+                  <c:v>0.166666666666667</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.302356011962149</c:v>
+                  <c:v>0.178571428571429</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.321257807999922</c:v>
+                  <c:v>0.185</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.369363593889636</c:v>
+                  <c:v>0.2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.415392897993352</c:v>
+                  <c:v>0.212765957446808</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.474527504585557</c:v>
+                  <c:v>0.227272727272727</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.524285038817918</c:v>
+                  <c:v>0.238095238095238</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.585699763462427</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.686172536550428</c:v>
+                  <c:v>0.266666666666667</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.828253787040738</c:v>
+                  <c:v>0.285714285714286</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>1.04453979786481</c:v>
+                  <c:v>0.307692307692308</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>1.41370849400737</c:v>
+                  <c:v>0.333333333333333</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -659,11 +646,229 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="49855205"/>
-        <c:axId val="51720315"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1/(V-A)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="ff420e"/>
+            </a:solidFill>
+            <a:ln w="28800">
+              <a:solidFill>
+                <a:srgbClr val="ff420e"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
+            <c:txPr>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:latin typeface="Arial"/>
+                  </a:defRPr>
+                </a:pPr>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showLeaderLines val="0"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$I$2:$I$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>0.000352148962352698</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.00130342858125705</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.00849564551485895</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0128687939938936</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.0218783148491767</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0440385859992941</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.0636644246928005</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.0933937082076311</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.103014626142723</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.129746122812774</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.175212375625125</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.203775578136928</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.252693752957386</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.269733762119723</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.302356011962149</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.321257807999923</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.369363593889636</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.415392897993352</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.474527504585557</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.524285038817918</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.585699763462427</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.686172536550427</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.828253787040737</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.04453979786481</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.41370849400737</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$B$2:$B$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>2.77</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.26</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>197</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>452</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>730</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1255</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1450</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2050</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3280</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4170</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5925</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6520</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>7835</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8550</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10590</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12430</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>14860</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>16900</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>19130</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>23000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>27550</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>33000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>40000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="62856448"/>
+        <c:axId val="61312878"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="49855205"/>
+        <c:axId val="62856448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -700,12 +905,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="51720315"/>
+        <c:crossAx val="61312878"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="51720315"/>
+        <c:axId val="61312878"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -742,7 +947,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49855205"/>
+        <c:crossAx val="62856448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -794,16 +999,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>36360</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>713520</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>67320</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>48240</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>204840</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>118800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -811,7 +1016,7 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6350760" y="0"/>
+        <a:off x="713520" y="0"/>
         <a:ext cx="7619040" cy="6458400"/>
       </xdr:xfrm>
       <a:graphic>
@@ -826,17 +1031,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:H18" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
-  <autoFilter ref="A1:H18"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:I18" headerRowCount="1" totalsRowCount="0" totalsRowShown="0">
+  <autoFilter ref="A1:I18"/>
+  <tableColumns count="9">
     <tableColumn id="1" name="NkT"/>
     <tableColumn id="2" name="P"/>
     <tableColumn id="3" name="V"/>
     <tableColumn id="4" name="V-A"/>
     <tableColumn id="5" name="PV"/>
-    <tableColumn id="6" name="ratio"/>
-    <tableColumn id="7" name="1/V"/>
-    <tableColumn id="8" name="1/(V-A)"/>
+    <tableColumn id="6" name="P(V-A)"/>
+    <tableColumn id="7" name="ratio"/>
+    <tableColumn id="8" name="1/V"/>
+    <tableColumn id="9" name="1/(V-A)"/>
   </tableColumns>
 </table>
 </file>
@@ -846,17 +1052,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F32" activeCellId="0" sqref="F32"/>
+      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="1" style="0" width="8.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="9" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="1" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="11.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="0" width="8.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -887,6 +1093,9 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -899,7 +1108,7 @@
         <v>2842</v>
       </c>
       <c r="D2" s="0" t="n">
-        <f aca="false">C2-$I$2</f>
+        <f aca="false">C2-$K$2</f>
         <v>2839.70735940559</v>
       </c>
       <c r="E2" s="0" t="n">
@@ -907,18 +1116,22 @@
         <v>7872.34</v>
       </c>
       <c r="F2" s="0" t="n">
+        <f aca="false">B2*D2</f>
+        <v>7865.98938555349</v>
+      </c>
+      <c r="G2" s="0" t="n">
         <f aca="false">E2/A2</f>
         <v>1.00927435897436</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="H2" s="0" t="n">
         <f aca="false">1/C2</f>
         <v>0.000351864883884588</v>
       </c>
-      <c r="H2" s="0" t="n">
-        <f aca="false">1/(C2-$I$2)</f>
+      <c r="I2" s="0" t="n">
+        <f aca="false">1/(C2-$K$2)</f>
         <v>0.000352148962352698</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="K2" s="0" t="n">
         <f aca="false">4/3*0.065^3*1993*PI()</f>
         <v>2.292640594409</v>
       </c>
@@ -934,7 +1147,7 @@
         <v>769.5</v>
       </c>
       <c r="D3" s="0" t="n">
-        <f aca="false">C3-$I$2</f>
+        <f aca="false">C3-$K$2</f>
         <v>767.207359405591</v>
       </c>
       <c r="E3" s="0" t="n">
@@ -942,15 +1155,19 @@
         <v>7895.07</v>
       </c>
       <c r="F3" s="0" t="n">
+        <f aca="false">B3*D3</f>
+        <v>7871.54750750136</v>
+      </c>
+      <c r="G3" s="0" t="n">
         <f aca="false">E3/A3</f>
         <v>1.02533376623377</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="H3" s="0" t="n">
         <f aca="false">1/C3</f>
         <v>0.00129954515919428</v>
       </c>
-      <c r="H3" s="0" t="n">
-        <f aca="false">1/(C3-$I$2)</f>
+      <c r="I3" s="0" t="n">
+        <f aca="false">1/(C3-$K$2)</f>
         <v>0.00130342858125705</v>
       </c>
     </row>
@@ -965,7 +1182,7 @@
         <v>120</v>
       </c>
       <c r="D4" s="0" t="n">
-        <f aca="false">C4-$I$2</f>
+        <f aca="false">C4-$K$2</f>
         <v>117.707359405591</v>
       </c>
       <c r="E4" s="0" t="n">
@@ -973,15 +1190,19 @@
         <v>8400</v>
       </c>
       <c r="F4" s="0" t="n">
+        <f aca="false">B4*D4</f>
+        <v>8239.51515839137</v>
+      </c>
+      <c r="G4" s="0" t="n">
         <f aca="false">E4/A4</f>
         <v>1.09090909090909</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="H4" s="0" t="n">
         <f aca="false">1/C4</f>
         <v>0.00833333333333333</v>
       </c>
-      <c r="H4" s="0" t="n">
-        <f aca="false">1/(C4-$I$2)</f>
+      <c r="I4" s="0" t="n">
+        <f aca="false">1/(C4-$K$2)</f>
         <v>0.00849564551485895</v>
       </c>
     </row>
@@ -996,7 +1217,7 @@
         <v>80</v>
       </c>
       <c r="D5" s="0" t="n">
-        <f aca="false">C5-$I$2</f>
+        <f aca="false">C5-$K$2</f>
         <v>77.707359405591</v>
       </c>
       <c r="E5" s="0" t="n">
@@ -1004,15 +1225,19 @@
         <v>8800</v>
       </c>
       <c r="F5" s="0" t="n">
+        <f aca="false">B5*D5</f>
+        <v>8547.80953461501</v>
+      </c>
+      <c r="G5" s="0" t="n">
         <f aca="false">E5/A5</f>
         <v>1.14285714285714</v>
       </c>
-      <c r="G5" s="0" t="n">
+      <c r="H5" s="0" t="n">
         <f aca="false">1/C5</f>
         <v>0.0125</v>
       </c>
-      <c r="H5" s="0" t="n">
-        <f aca="false">1/(C5-$I$2)</f>
+      <c r="I5" s="0" t="n">
+        <f aca="false">1/(C5-$K$2)</f>
         <v>0.0128687939938936</v>
       </c>
     </row>
@@ -1027,7 +1252,7 @@
         <v>48</v>
       </c>
       <c r="D6" s="0" t="n">
-        <f aca="false">C6-$I$2</f>
+        <f aca="false">C6-$K$2</f>
         <v>45.707359405591</v>
       </c>
       <c r="E6" s="0" t="n">
@@ -1035,15 +1260,19 @@
         <v>9456</v>
       </c>
       <c r="F6" s="0" t="n">
+        <f aca="false">B6*D6</f>
+        <v>9004.34980290143</v>
+      </c>
+      <c r="G6" s="0" t="n">
         <f aca="false">E6/A6</f>
         <v>1.22805194805195</v>
       </c>
-      <c r="G6" s="0" t="n">
+      <c r="H6" s="0" t="n">
         <f aca="false">1/C6</f>
         <v>0.0208333333333333</v>
       </c>
-      <c r="H6" s="0" t="n">
-        <f aca="false">1/(C6-$I$2)</f>
+      <c r="I6" s="0" t="n">
+        <f aca="false">1/(C6-$K$2)</f>
         <v>0.0218783148491767</v>
       </c>
     </row>
@@ -1058,7 +1287,7 @@
         <v>25</v>
       </c>
       <c r="D7" s="0" t="n">
-        <f aca="false">C7-$I$2</f>
+        <f aca="false">C7-$K$2</f>
         <v>22.707359405591</v>
       </c>
       <c r="E7" s="0" t="n">
@@ -1066,15 +1295,19 @@
         <v>11300</v>
       </c>
       <c r="F7" s="0" t="n">
+        <f aca="false">B7*D7</f>
+        <v>10263.7264513271</v>
+      </c>
+      <c r="G7" s="0" t="n">
         <f aca="false">E7/A7</f>
         <v>1.44871794871795</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="H7" s="0" t="n">
         <f aca="false">1/C7</f>
         <v>0.04</v>
       </c>
-      <c r="H7" s="0" t="n">
-        <f aca="false">1/(C7-$I$2)</f>
+      <c r="I7" s="0" t="n">
+        <f aca="false">1/(C7-$K$2)</f>
         <v>0.0440385859992941</v>
       </c>
     </row>
@@ -1089,7 +1322,7 @@
         <v>18</v>
       </c>
       <c r="D8" s="0" t="n">
-        <f aca="false">C8-$I$2</f>
+        <f aca="false">C8-$K$2</f>
         <v>15.707359405591</v>
       </c>
       <c r="E8" s="0" t="n">
@@ -1097,15 +1330,19 @@
         <v>13140</v>
       </c>
       <c r="F8" s="0" t="n">
+        <f aca="false">B8*D8</f>
+        <v>11466.3723660814</v>
+      </c>
+      <c r="G8" s="0" t="n">
         <f aca="false">E8/A8</f>
         <v>1.70649350649351</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="H8" s="0" t="n">
         <f aca="false">1/C8</f>
         <v>0.0555555555555556</v>
       </c>
-      <c r="H8" s="0" t="n">
-        <f aca="false">1/(C8-$I$2)</f>
+      <c r="I8" s="0" t="n">
+        <f aca="false">1/(C8-$K$2)</f>
         <v>0.0636644246928005</v>
       </c>
     </row>
@@ -1120,7 +1357,7 @@
         <v>13</v>
       </c>
       <c r="D9" s="0" t="n">
-        <f aca="false">C9-$I$2</f>
+        <f aca="false">C9-$K$2</f>
         <v>10.707359405591</v>
       </c>
       <c r="E9" s="0" t="n">
@@ -1128,15 +1365,19 @@
         <v>16315</v>
       </c>
       <c r="F9" s="0" t="n">
+        <f aca="false">B9*D9</f>
+        <v>13437.7360540167</v>
+      </c>
+      <c r="G9" s="0" t="n">
         <f aca="false">E9/A9</f>
         <v>2.11883116883117</v>
       </c>
-      <c r="G9" s="0" t="n">
+      <c r="H9" s="0" t="n">
         <f aca="false">1/C9</f>
         <v>0.0769230769230769</v>
       </c>
-      <c r="H9" s="0" t="n">
-        <f aca="false">1/(C9-$I$2)</f>
+      <c r="I9" s="0" t="n">
+        <f aca="false">1/(C9-$K$2)</f>
         <v>0.0933937082076311</v>
       </c>
     </row>
@@ -1151,7 +1392,7 @@
         <v>12</v>
       </c>
       <c r="D10" s="0" t="n">
-        <f aca="false">C10-$I$2</f>
+        <f aca="false">C10-$K$2</f>
         <v>9.707359405591</v>
       </c>
       <c r="E10" s="0" t="n">
@@ -1159,15 +1400,19 @@
         <v>17400</v>
       </c>
       <c r="F10" s="0" t="n">
+        <f aca="false">B10*D10</f>
+        <v>14075.671138107</v>
+      </c>
+      <c r="G10" s="0" t="n">
         <f aca="false">E10/A10</f>
         <v>2.25974025974026</v>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="H10" s="0" t="n">
         <f aca="false">1/C10</f>
         <v>0.0833333333333333</v>
       </c>
-      <c r="H10" s="0" t="n">
-        <f aca="false">1/(C10-$I$2)</f>
+      <c r="I10" s="0" t="n">
+        <f aca="false">1/(C10-$K$2)</f>
         <v>0.103014626142723</v>
       </c>
     </row>
@@ -1182,7 +1427,7 @@
         <v>10</v>
       </c>
       <c r="D11" s="0" t="n">
-        <f aca="false">C11-$I$2</f>
+        <f aca="false">C11-$K$2</f>
         <v>7.707359405591</v>
       </c>
       <c r="E11" s="0" t="n">
@@ -1190,15 +1435,19 @@
         <v>20500</v>
       </c>
       <c r="F11" s="0" t="n">
+        <f aca="false">B11*D11</f>
+        <v>15800.0867814616</v>
+      </c>
+      <c r="G11" s="0" t="n">
         <f aca="false">E11/A11</f>
         <v>2.66233766233766</v>
       </c>
-      <c r="G11" s="0" t="n">
+      <c r="H11" s="0" t="n">
         <f aca="false">1/C11</f>
         <v>0.1</v>
       </c>
-      <c r="H11" s="0" t="n">
-        <f aca="false">1/(C11-$I$2)</f>
+      <c r="I11" s="0" t="n">
+        <f aca="false">1/(C11-$K$2)</f>
         <v>0.129746122812774</v>
       </c>
     </row>
@@ -1213,7 +1462,7 @@
         <v>8</v>
       </c>
       <c r="D12" s="0" t="n">
-        <f aca="false">C12-$I$2</f>
+        <f aca="false">C12-$K$2</f>
         <v>5.707359405591</v>
       </c>
       <c r="E12" s="0" t="n">
@@ -1221,15 +1470,19 @@
         <v>26240</v>
       </c>
       <c r="F12" s="0" t="n">
+        <f aca="false">B12*D12</f>
+        <v>18720.1388503385</v>
+      </c>
+      <c r="G12" s="0" t="n">
         <f aca="false">E12/A12</f>
         <v>3.40779220779221</v>
       </c>
-      <c r="G12" s="0" t="n">
+      <c r="H12" s="0" t="n">
         <f aca="false">1/C12</f>
         <v>0.125</v>
       </c>
-      <c r="H12" s="0" t="n">
-        <f aca="false">1/(C12-$I$2)</f>
+      <c r="I12" s="0" t="n">
+        <f aca="false">1/(C12-$K$2)</f>
         <v>0.175212375625125</v>
       </c>
     </row>
@@ -1244,7 +1497,7 @@
         <v>7.2</v>
       </c>
       <c r="D13" s="0" t="n">
-        <f aca="false">C13-$I$2</f>
+        <f aca="false">C13-$K$2</f>
         <v>4.907359405591</v>
       </c>
       <c r="E13" s="0" t="n">
@@ -1252,15 +1505,19 @@
         <v>30024</v>
       </c>
       <c r="F13" s="0" t="n">
+        <f aca="false">B13*D13</f>
+        <v>20463.6887213145</v>
+      </c>
+      <c r="G13" s="0" t="n">
         <f aca="false">E13/A13</f>
         <v>3.89922077922078</v>
       </c>
-      <c r="G13" s="0" t="n">
+      <c r="H13" s="0" t="n">
         <f aca="false">1/C13</f>
         <v>0.138888888888889</v>
       </c>
-      <c r="H13" s="0" t="n">
-        <f aca="false">1/(C13-$I$2)</f>
+      <c r="I13" s="0" t="n">
+        <f aca="false">1/(C13-$K$2)</f>
         <v>0.203775578136928</v>
       </c>
     </row>
@@ -1275,7 +1532,7 @@
         <v>6.25</v>
       </c>
       <c r="D14" s="0" t="n">
-        <f aca="false">C14-$I$2</f>
+        <f aca="false">C14-$K$2</f>
         <v>3.957359405591</v>
       </c>
       <c r="E14" s="0" t="n">
@@ -1283,15 +1540,19 @@
         <v>37031.25</v>
       </c>
       <c r="F14" s="0" t="n">
+        <f aca="false">B14*D14</f>
+        <v>23447.3544781267</v>
+      </c>
+      <c r="G14" s="0" t="n">
         <f aca="false">E14/A14</f>
         <v>4.80925324675325</v>
       </c>
-      <c r="G14" s="0" t="n">
+      <c r="H14" s="0" t="n">
         <f aca="false">1/C14</f>
         <v>0.16</v>
       </c>
-      <c r="H14" s="0" t="n">
-        <f aca="false">1/(C14-$I$2)</f>
+      <c r="I14" s="0" t="n">
+        <f aca="false">1/(C14-$K$2)</f>
         <v>0.252693752957386</v>
       </c>
     </row>
@@ -1306,7 +1567,7 @@
         <v>6</v>
       </c>
       <c r="D15" s="0" t="n">
-        <f aca="false">C15-$I$2</f>
+        <f aca="false">C15-$K$2</f>
         <v>3.707359405591</v>
       </c>
       <c r="E15" s="0" t="n">
@@ -1314,15 +1575,19 @@
         <v>39120</v>
       </c>
       <c r="F15" s="0" t="n">
+        <f aca="false">B15*D15</f>
+        <v>24171.9833244533</v>
+      </c>
+      <c r="G15" s="0" t="n">
         <f aca="false">E15/A15</f>
         <v>5.08051948051948</v>
       </c>
-      <c r="G15" s="0" t="n">
+      <c r="H15" s="0" t="n">
         <f aca="false">1/C15</f>
         <v>0.166666666666667</v>
       </c>
-      <c r="H15" s="0" t="n">
-        <f aca="false">1/(C15-$I$2)</f>
+      <c r="I15" s="0" t="n">
+        <f aca="false">1/(C15-$K$2)</f>
         <v>0.269733762119723</v>
       </c>
     </row>
@@ -1337,7 +1602,7 @@
         <v>5.6</v>
       </c>
       <c r="D16" s="0" t="n">
-        <f aca="false">C16-$I$2</f>
+        <f aca="false">C16-$K$2</f>
         <v>3.307359405591</v>
       </c>
       <c r="E16" s="0" t="n">
@@ -1345,15 +1610,19 @@
         <v>43876</v>
       </c>
       <c r="F16" s="0" t="n">
+        <f aca="false">B16*D16</f>
+        <v>25913.1609428055</v>
+      </c>
+      <c r="G16" s="0" t="n">
         <f aca="false">E16/A16</f>
         <v>5.69818181818182</v>
       </c>
-      <c r="G16" s="0" t="n">
+      <c r="H16" s="0" t="n">
         <f aca="false">1/C16</f>
         <v>0.178571428571429</v>
       </c>
-      <c r="H16" s="0" t="n">
-        <f aca="false">1/(C16-$I$2)</f>
+      <c r="I16" s="0" t="n">
+        <f aca="false">1/(C16-$K$2)</f>
         <v>0.302356011962149</v>
       </c>
     </row>
@@ -1369,7 +1638,7 @@
         <v>5.40540540540541</v>
       </c>
       <c r="D17" s="0" t="n">
-        <f aca="false">C17-$I$2</f>
+        <f aca="false">C17-$K$2</f>
         <v>3.11276481099641</v>
       </c>
       <c r="E17" s="0" t="n">
@@ -1377,16 +1646,20 @@
         <v>46216.2162162162</v>
       </c>
       <c r="F17" s="0" t="n">
+        <f aca="false">B17*D17</f>
+        <v>26614.1391340193</v>
+      </c>
+      <c r="G17" s="0" t="n">
         <f aca="false">E17/A17</f>
-        <v>6.00210600210601</v>
-      </c>
-      <c r="G17" s="0" t="n">
+        <v>6.002106002106</v>
+      </c>
+      <c r="H17" s="0" t="n">
         <f aca="false">1/C17</f>
         <v>0.185</v>
       </c>
-      <c r="H17" s="0" t="n">
-        <f aca="false">1/(C17-$I$2)</f>
-        <v>0.321257807999922</v>
+      <c r="I17" s="0" t="n">
+        <f aca="false">1/(C17-$K$2)</f>
+        <v>0.321257807999923</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1400,7 +1673,7 @@
         <v>5</v>
       </c>
       <c r="D18" s="0" t="n">
-        <f aca="false">C18-$I$2</f>
+        <f aca="false">C18-$K$2</f>
         <v>2.707359405591</v>
       </c>
       <c r="E18" s="0" t="n">
@@ -1408,15 +1681,19 @@
         <v>52950</v>
       </c>
       <c r="F18" s="0" t="n">
+        <f aca="false">B18*D18</f>
+        <v>28670.9361052087</v>
+      </c>
+      <c r="G18" s="0" t="n">
         <f aca="false">E18/A18</f>
         <v>6.87662337662338</v>
       </c>
-      <c r="G18" s="0" t="n">
+      <c r="H18" s="0" t="n">
         <f aca="false">1/C18</f>
         <v>0.2</v>
       </c>
-      <c r="H18" s="0" t="n">
-        <f aca="false">1/(C18-$I$2)</f>
+      <c r="I18" s="0" t="n">
+        <f aca="false">1/(C18-$K$2)</f>
         <v>0.369363593889636</v>
       </c>
     </row>
@@ -1431,7 +1708,7 @@
         <v>4.7</v>
       </c>
       <c r="D19" s="0" t="n">
-        <f aca="false">C19-$I$2</f>
+        <f aca="false">C19-$K$2</f>
         <v>2.407359405591</v>
       </c>
       <c r="E19" s="0" t="n">
@@ -1439,15 +1716,19 @@
         <v>58421</v>
       </c>
       <c r="F19" s="0" t="n">
+        <f aca="false">B19*D19</f>
+        <v>29923.4774114961</v>
+      </c>
+      <c r="G19" s="0" t="n">
         <f aca="false">E19/A19</f>
         <v>7.58714285714286</v>
       </c>
-      <c r="G19" s="0" t="n">
+      <c r="H19" s="0" t="n">
         <f aca="false">1/C19</f>
         <v>0.212765957446808</v>
       </c>
-      <c r="H19" s="0" t="n">
-        <f aca="false">1/(C19-$I$2)</f>
+      <c r="I19" s="0" t="n">
+        <f aca="false">1/(C19-$K$2)</f>
         <v>0.415392897993352</v>
       </c>
     </row>
@@ -1462,7 +1743,7 @@
         <v>4.4</v>
       </c>
       <c r="D20" s="0" t="n">
-        <f aca="false">C20-$I$2</f>
+        <f aca="false">C20-$K$2</f>
         <v>2.107359405591</v>
       </c>
       <c r="E20" s="0" t="n">
@@ -1470,15 +1751,19 @@
         <v>65384</v>
       </c>
       <c r="F20" s="0" t="n">
+        <f aca="false">B20*D20</f>
+        <v>31315.3607670823</v>
+      </c>
+      <c r="G20" s="0" t="n">
         <f aca="false">E20/A20</f>
         <v>8.49142857142857</v>
       </c>
-      <c r="G20" s="0" t="n">
+      <c r="H20" s="0" t="n">
         <f aca="false">1/C20</f>
         <v>0.227272727272727</v>
       </c>
-      <c r="H20" s="0" t="n">
-        <f aca="false">1/(C20-$I$2)</f>
+      <c r="I20" s="0" t="n">
+        <f aca="false">1/(C20-$K$2)</f>
         <v>0.474527504585557</v>
       </c>
     </row>
@@ -1493,7 +1778,7 @@
         <v>4.2</v>
       </c>
       <c r="D21" s="0" t="n">
-        <f aca="false">C21-$I$2</f>
+        <f aca="false">C21-$K$2</f>
         <v>1.907359405591</v>
       </c>
       <c r="E21" s="0" t="n">
@@ -1501,15 +1786,19 @@
         <v>70980</v>
       </c>
       <c r="F21" s="0" t="n">
+        <f aca="false">B21*D21</f>
+        <v>32234.3739544879</v>
+      </c>
+      <c r="G21" s="0" t="n">
         <f aca="false">E21/A21</f>
         <v>9.21818181818182</v>
       </c>
-      <c r="G21" s="0" t="n">
+      <c r="H21" s="0" t="n">
         <f aca="false">1/C21</f>
         <v>0.238095238095238</v>
       </c>
-      <c r="H21" s="0" t="n">
-        <f aca="false">1/(C21-$I$2)</f>
+      <c r="I21" s="0" t="n">
+        <f aca="false">1/(C21-$K$2)</f>
         <v>0.524285038817918</v>
       </c>
     </row>
@@ -1524,7 +1813,7 @@
         <v>4</v>
       </c>
       <c r="D22" s="0" t="n">
-        <f aca="false">C22-$I$2</f>
+        <f aca="false">C22-$K$2</f>
         <v>1.707359405591</v>
       </c>
       <c r="E22" s="0" t="n">
@@ -1532,15 +1821,19 @@
         <v>76520</v>
       </c>
       <c r="F22" s="0" t="n">
+        <f aca="false">B22*D22</f>
+        <v>32661.7854289558</v>
+      </c>
+      <c r="G22" s="0" t="n">
         <f aca="false">E22/A22</f>
         <v>9.93766233766234</v>
       </c>
-      <c r="G22" s="0" t="n">
+      <c r="H22" s="0" t="n">
         <f aca="false">1/C22</f>
         <v>0.25</v>
       </c>
-      <c r="H22" s="0" t="n">
-        <f aca="false">1/(C22-$I$2)</f>
+      <c r="I22" s="0" t="n">
+        <f aca="false">1/(C22-$K$2)</f>
         <v>0.585699763462427</v>
       </c>
     </row>
@@ -1555,7 +1848,7 @@
         <v>3.75</v>
       </c>
       <c r="D23" s="0" t="n">
-        <f aca="false">C23-$I$2</f>
+        <f aca="false">C23-$K$2</f>
         <v>1.457359405591</v>
       </c>
       <c r="E23" s="0" t="n">
@@ -1563,16 +1856,20 @@
         <v>86250</v>
       </c>
       <c r="F23" s="0" t="n">
+        <f aca="false">B23*D23</f>
+        <v>33519.266328593</v>
+      </c>
+      <c r="G23" s="0" t="n">
         <f aca="false">E23/A23</f>
         <v>11.2012987012987</v>
       </c>
-      <c r="G23" s="0" t="n">
+      <c r="H23" s="0" t="n">
         <f aca="false">1/C23</f>
         <v>0.266666666666667</v>
       </c>
-      <c r="H23" s="0" t="n">
-        <f aca="false">1/(C23-$I$2)</f>
-        <v>0.686172536550428</v>
+      <c r="I23" s="0" t="n">
+        <f aca="false">1/(C23-$K$2)</f>
+        <v>0.686172536550427</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1586,7 +1883,7 @@
         <v>3.5</v>
       </c>
       <c r="D24" s="0" t="n">
-        <f aca="false">C24-$I$2</f>
+        <f aca="false">C24-$K$2</f>
         <v>1.207359405591</v>
       </c>
       <c r="E24" s="0" t="n">
@@ -1594,16 +1891,20 @@
         <v>96425</v>
       </c>
       <c r="F24" s="0" t="n">
+        <f aca="false">B24*D24</f>
+        <v>33262.7516240321</v>
+      </c>
+      <c r="G24" s="0" t="n">
         <f aca="false">E24/A24</f>
         <v>12.5227272727273</v>
       </c>
-      <c r="G24" s="0" t="n">
+      <c r="H24" s="0" t="n">
         <f aca="false">1/C24</f>
         <v>0.285714285714286</v>
       </c>
-      <c r="H24" s="0" t="n">
-        <f aca="false">1/(C24-$I$2)</f>
-        <v>0.828253787040738</v>
+      <c r="I24" s="0" t="n">
+        <f aca="false">1/(C24-$K$2)</f>
+        <v>0.828253787040737</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1617,23 +1918,27 @@
         <v>3.25</v>
       </c>
       <c r="D25" s="0" t="n">
-        <f aca="false">C25-$I$2</f>
-        <v>0.957359405591</v>
+        <f aca="false">C25-$K$2</f>
+        <v>0.957359405591001</v>
       </c>
       <c r="E25" s="0" t="n">
         <f aca="false">B25*C25</f>
         <v>107250</v>
       </c>
       <c r="F25" s="0" t="n">
+        <f aca="false">B25*D25</f>
+        <v>31592.860384503</v>
+      </c>
+      <c r="G25" s="0" t="n">
         <f aca="false">E25/A25</f>
         <v>13.9285714285714</v>
       </c>
-      <c r="G25" s="0" t="n">
+      <c r="H25" s="0" t="n">
         <f aca="false">1/C25</f>
         <v>0.307692307692308</v>
       </c>
-      <c r="H25" s="0" t="n">
-        <f aca="false">1/(C25-$I$2)</f>
+      <c r="I25" s="0" t="n">
+        <f aca="false">1/(C25-$K$2)</f>
         <v>1.04453979786481</v>
       </c>
     </row>
@@ -1648,7 +1953,7 @@
         <v>3</v>
       </c>
       <c r="D26" s="0" t="n">
-        <f aca="false">C26-$I$2</f>
+        <f aca="false">C26-$K$2</f>
         <v>0.707359405591001</v>
       </c>
       <c r="E26" s="0" t="n">
@@ -1656,15 +1961,19 @@
         <v>120000</v>
       </c>
       <c r="F26" s="0" t="n">
+        <f aca="false">B26*D26</f>
+        <v>28294.37622364</v>
+      </c>
+      <c r="G26" s="0" t="n">
         <f aca="false">E26/A26</f>
         <v>15.5844155844156</v>
       </c>
-      <c r="G26" s="0" t="n">
+      <c r="H26" s="0" t="n">
         <f aca="false">1/C26</f>
         <v>0.333333333333333</v>
       </c>
-      <c r="H26" s="0" t="n">
-        <f aca="false">1/(C26-$I$2)</f>
+      <c r="I26" s="0" t="n">
+        <f aca="false">1/(C26-$K$2)</f>
         <v>1.41370849400737</v>
       </c>
     </row>
@@ -1676,9 +1985,8 @@
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
-  <drawing r:id="rId1"/>
   <tableParts>
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1691,7 +1999,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J15" activeCellId="0" sqref="J15"/>
+      <selection pane="topLeft" activeCell="M13" activeCellId="0" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1706,5 +2014,6 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>